<commit_message>
Updated salinity, ck project structure in Plot-Figure folder and script
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Salinity_Estimation/0-Dataset/training_2016_2017_test_2018_2019_comparing_old_model/Q_river_Class_splitted/SALINITY_Q_RIVER_CLASS_SPLIT.xlsx
+++ b/Parameters-Estimation/Salinity_Estimation/0-Dataset/training_2016_2017_test_2018_2019_comparing_old_model/Q_river_Class_splitted/SALINITY_Q_RIVER_CLASS_SPLIT.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_Estuarine Box Model\Experiments\Parameters-Estimation\Salinity_Estimation\0-Dataset\training_2016_2017_test_2018_2019_comparing_old_model\Q_river_Class_splitted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6820B6D6-990E-4E1A-8D38-327FFF7C3BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB97984-059A-4994-B49F-8913AEA169F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BD1785B-D056-4443-A1F9-0A596533BA3E}"/>
+    <workbookView xWindow="-20610" yWindow="4455" windowWidth="20730" windowHeight="11160" xr2:uid="{0BD1785B-D056-4443-A1F9-0A596533BA3E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Salinity_Q_river_splitted" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>